<commit_message>
feat: add to support the allocating only allocator
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/alloc_only_allocator.xlsx
+++ b/libalconcurrent/doc/alloc_only_allocator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C32874-4680-4A31-917A-1713F678B360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299AE698-28FE-424D-AAB8-5926FD13A0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>allocate_by_mmap()でOSからメモリ領域を確保</t>
     <rPh sb="26" eb="28">
@@ -123,16 +123,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>参照先候補スタックのヘッドへのポインタ</t>
-    <rPh sb="0" eb="3">
-      <t>サンショウサキ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>コウホ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>参照先候補スタックリストとしての次へのポインタ</t>
     <rPh sb="0" eb="3">
       <t>サンショウサキ</t>
@@ -146,33 +136,47 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>※スレッド終了により未参照領域が</t>
-    <rPh sb="5" eb="7">
-      <t>シュウリョウ</t>
+    <t>free_room</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>chopped_size_</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>offset_into_the_allocated_memory_</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(アライメントの合わせ込みのためのパディング領域)</t>
+    <rPh sb="8" eb="9">
+      <t>ア</t>
     </rPh>
-    <rPh sb="10" eb="13">
-      <t>ミサンショウ</t>
+    <rPh sb="11" eb="12">
+      <t>コ</t>
     </rPh>
-    <rPh sb="13" eb="15">
+    <rPh sb="22" eb="24">
       <t>リョウイキ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>　発生した場合に空き領域が期待され</t>
-    <rPh sb="8" eb="9">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>リョウイキ</t>
-    </rPh>
-    <rPh sb="13" eb="15">
-      <t>キタイ</t>
+    <t>tail_padding</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バックトレース情報(コンパイルオプション)</t>
+    <rPh sb="7" eb="9">
+      <t>ジョウホウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>　るため、それを保持するリスト</t>
+    <t>バックトレース情報(コンパイルオプション)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x???</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -221,7 +225,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -279,11 +283,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -298,6 +317,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1009,14 +1032,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1032,8 +1055,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8429625" y="4629150"/>
-          <a:ext cx="219075" cy="285750"/>
+          <a:off x="8429626" y="3962400"/>
+          <a:ext cx="209550" cy="952500"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1124,13 +1147,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>132521</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1146,8 +1169,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8477250" y="9439274"/>
-          <a:ext cx="180975" cy="694497"/>
+          <a:off x="8477250" y="8715375"/>
+          <a:ext cx="409575" cy="3085271"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1244,7 +1267,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1464,7 +1487,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1563,56 +1586,916 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2000250</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>1933575</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2371725</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="左中かっこ 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ACA4A3E-322D-C8A8-B206-095EEA061D33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2619375" y="9553575"/>
+          <a:ext cx="438150" cy="2105025"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 40942"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>219074</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="直線矢印コネクタ 14">
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="左中かっこ 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD2A8C2D-11EE-445E-9B11-50758C99A945}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9047406C-92D1-49A5-94D0-819A7962495F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2686050" y="2400300"/>
-          <a:ext cx="2209800" cy="6781800"/>
+          <a:off x="4248150" y="9772649"/>
+          <a:ext cx="438150" cy="923925"/>
         </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 40942"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2581275</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="975139" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="テキスト ボックス 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24AAAA85-B7BD-C799-8D48-D6976E3E2975}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3267075" y="9848850"/>
+          <a:ext cx="975139" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>room_boader</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1066254" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="テキスト ボックス 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5C4BD0F-ABC2-4C09-4F99-63FAA10B68DB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1619250" y="10448925"/>
+          <a:ext cx="1066254" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>chopped_room</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>219076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="左中かっこ 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{641EA408-75A7-4B90-98BD-2FDF7EE13FF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4257675" y="10506077"/>
+          <a:ext cx="438150" cy="904874"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 40942"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2409825</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1225015" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="テキスト ボックス 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B1C4F2B-0E84-488B-8ED6-24C7D1E85D62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="10810875"/>
+          <a:ext cx="1225015" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>allocated memory</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>28577</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="左中かっこ 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9BEF792-F775-4C69-B1C5-F20EAAF388D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4257675" y="11458577"/>
+          <a:ext cx="438150" cy="190498"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 40942"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2409825</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1313180" cy="1445011"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="テキスト ボックス 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4D3F358-EB5A-4CF9-838F-908F40C2A4B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="11401425"/>
+          <a:ext cx="1313180" cy="1445011"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>tail_padding</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>room_boader</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>アライメントを</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>合わせるための</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>パディング領域</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>（必ず確保する）</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1866900</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2143125</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="右中かっこ 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{320D5625-31A0-1704-E65D-297B2AE3A297}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11668125" y="9563100"/>
+          <a:ext cx="276225" cy="2114550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 49712"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2181225</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1141531" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="テキスト ボックス 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93AE9C2C-A4B7-4D57-B1AB-89594ED32279}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11982450" y="10477500"/>
+          <a:ext cx="1141531" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>= chopped_size_</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4070666" cy="328423"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="テキスト ボックス 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C634D08-B4B2-4C3D-A470-06C2C1AD63FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8601075" y="4572000"/>
+          <a:ext cx="4070666" cy="328423"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>次の空き領域へオフセット </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>= chamber</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>先頭からのオフセット</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="フリーフォーム: 図形 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FFB56D4-F66B-47EC-9B01-D0B64AF56EEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9163050" y="9629775"/>
+          <a:ext cx="409575" cy="933450"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
+            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
+            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
+            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
+            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
+            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
+            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
+            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="200025" h="514350">
+              <a:moveTo>
+                <a:pt x="28575" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="200025" y="114300"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="200025" y="409575"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="133350" y="514350"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="514350"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
         <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4773486" cy="328423"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="テキスト ボックス 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72FB9630-2D62-532A-6496-70CD6F87D7C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9639300" y="9648825"/>
+          <a:ext cx="4773486" cy="328423"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
+          <a:scrgbClr r="0" g="0" b="0"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
         </a:fontRef>
       </xdr:style>
-    </xdr:cxnSp>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>offset_into_the_allocated_memory_</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>= room_boader</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>の</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>先頭からのオフセット</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2152,10 +3035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19FBDA2-FF85-45FB-B4CE-107905DAFA5C}">
-  <dimension ref="B2:N43"/>
+  <dimension ref="B2:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2205,26 +3088,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="B12" t="s">
-        <v>20</v>
-      </c>
-    </row>
     <row r="14" spans="2:14">
       <c r="E14" t="s">
         <v>0</v>
@@ -2251,7 +3114,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="4:5">
@@ -2266,10 +3129,15 @@
       <c r="D20">
         <v>32</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="21" spans="4:5">
-      <c r="E21" s="3"/>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="4:5">
       <c r="E22" s="3"/>
@@ -2287,7 +3155,9 @@
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="4:5">
-      <c r="E27" s="3"/>
+      <c r="E27" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="28" spans="4:5">
       <c r="E28" s="3"/>
@@ -2299,39 +3169,90 @@
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="4:5">
-      <c r="E31" s="4"/>
-    </row>
-    <row r="36" spans="5:5">
-      <c r="E36" s="1" t="s">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="4:5">
+      <c r="E32" s="4"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="E37" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="5:5">
-      <c r="E37" s="2" t="s">
+    <row r="38" spans="2:5">
+      <c r="E38" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="5:5">
-      <c r="E38" s="2" t="s">
+    <row r="39" spans="2:5">
+      <c r="E39" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="E40" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="E41" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="E42" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="E43" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="B44" s="8"/>
+      <c r="E44" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="E45" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="E47" s="7"/>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="E48" s="7"/>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="5:5">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="5:5">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="5:5">
+      <c r="E53" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="5:5">
-      <c r="E39" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="5:5">
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="5:5">
-      <c r="E41" s="7"/>
-    </row>
-    <row r="42" spans="5:5">
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="5:5">
-      <c r="E43" s="4"/>
+    <row r="54" spans="5:5">
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
feat: move internal header files to inc/internal
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/alloc_only_allocator.xlsx
+++ b/libalconcurrent/doc/alloc_only_allocator.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299AE698-28FE-424D-AAB8-5926FD13A0E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D60999D-425A-465A-82A4-A3B63A90C6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>allocate_by_mmap()でOSからメモリ領域を確保</t>
     <rPh sb="26" eb="28">
@@ -49,31 +48,6 @@
     <rPh sb="10" eb="12">
       <t>リョウイキ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>リザーブ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>次の空き領域へオフセット(size_t)</t>
-    <rPh sb="0" eb="1">
-      <t>ツギ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>リョウイキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>XXXX</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -177,6 +151,10 @@
   </si>
   <si>
     <t>0x???</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>std::atomic&lt;bool&gt; is_freeed_</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -342,695 +320,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="フリーフォーム: 図形 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D892899-EA0C-EDE3-7FAE-90AE3ED4E200}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7496175" y="2019300"/>
-          <a:ext cx="200025" cy="514350"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
-            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
-            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
-            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
-            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
-            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
-            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="200025" h="514350">
-              <a:moveTo>
-                <a:pt x="28575" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="200025" y="114300"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="200025" y="409575"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="133350" y="514350"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="514350"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="フリーフォーム: 図形 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D34F78C-536E-4AC4-8B16-C74A7C5C83BB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12458700" y="2028825"/>
-          <a:ext cx="504825" cy="1428750"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
-            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
-            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
-            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
-            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
-            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
-            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="200025" h="514350">
-              <a:moveTo>
-                <a:pt x="28575" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="200025" y="114300"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="200025" y="409575"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="133350" y="514350"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="514350"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="フリーフォーム: 図形 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6AA5B468-F3CE-40E3-892C-68C8ACCC3818}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12696825" y="2028825"/>
-          <a:ext cx="504825" cy="4514850"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
-            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
-            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
-            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
-            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
-            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
-            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="200025" h="514350">
-              <a:moveTo>
-                <a:pt x="28575" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="200025" y="114300"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="200025" y="409575"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="133350" y="514350"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="514350"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="フリーフォーム: 図形 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51A57660-A1A1-4258-AFD3-0539183F93BF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4067175" y="2019300"/>
-          <a:ext cx="200025" cy="514350"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
-            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
-            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
-            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
-            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
-            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
-            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="200025" h="514350">
-              <a:moveTo>
-                <a:pt x="28575" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="200025" y="114300"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="200025" y="409575"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="133350" y="514350"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="514350"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="フリーフォーム: 図形 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{028D4DB2-9D90-4C3F-9B75-A32906970FC9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16767727" y="8540198"/>
-          <a:ext cx="200025" cy="959954"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
-            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
-            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
-            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
-            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
-            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
-            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="200025" h="514350">
-              <a:moveTo>
-                <a:pt x="28575" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="200025" y="114300"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="200025" y="409575"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="133350" y="514350"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="514350"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="フリーフォーム: 図形 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FB37B88-D933-4838-85AD-D248647CB4E2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16735425" y="1790699"/>
-          <a:ext cx="752475" cy="6200775"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst>
-            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
-            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
-            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
-            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
-            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
-            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
-            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
-            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
-            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
-          </a:gdLst>
-          <a:ahLst/>
-          <a:cxnLst>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX0" y="connsiteY0"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX1" y="connsiteY1"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX2" y="connsiteY2"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX3" y="connsiteY3"/>
-            </a:cxn>
-            <a:cxn ang="0">
-              <a:pos x="connsiteX4" y="connsiteY4"/>
-            </a:cxn>
-          </a:cxnLst>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="200025" h="514350">
-              <a:moveTo>
-                <a:pt x="28575" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="200025" y="114300"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="200025" y="409575"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="133350" y="514350"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="0" y="514350"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>15</xdr:row>
@@ -1153,7 +442,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>132521</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1593,7 +882,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2371725</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1654,7 +943,7 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>219074</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1768,7 +1057,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>933450</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1066254" cy="264560"/>
@@ -1827,13 +1116,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>28577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>219076</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1888,7 +1177,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2409825</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1225015" cy="264560"/>
@@ -1947,13 +1236,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>28577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2008,7 +1297,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2409825</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1313180" cy="1445011"/>
@@ -2110,7 +1399,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2143125</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2165,7 +1454,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2181225</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1141531" cy="264560"/>
@@ -2309,7 +1598,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2496,6 +1785,89 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>219074</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="吹き出し: 角を丸めた四角形 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DF565FA-93D5-50DA-A99D-88153E84BDD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5514974" y="2124074"/>
+          <a:ext cx="3171825" cy="1019175"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRoundRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -28641"/>
+            <a:gd name="adj2" fmla="val 69977"/>
+            <a:gd name="adj3" fmla="val 16667"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>先頭領域は、コンパイル時に静的に確保した領域でもよいかも。</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>そうすれば、</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>constexpr</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>化できると思われる。</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2761,284 +2133,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:O41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19FBDA2-FF85-45FB-B4CE-107905DAFA5C}">
+  <dimension ref="B2:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
-  <cols>
-    <col min="3" max="3" width="35.125" customWidth="1"/>
-    <col min="4" max="4" width="3.875" customWidth="1"/>
-    <col min="5" max="5" width="15.375" customWidth="1"/>
-    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.125" customWidth="1"/>
-    <col min="13" max="13" width="3.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="2:12">
-      <c r="C5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12">
-      <c r="B8">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12">
-      <c r="B9">
-        <v>16</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9">
-        <v>16</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12">
-      <c r="B10">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12">
-      <c r="B11">
-        <v>32</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="E11">
-        <v>32</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="2:12">
-      <c r="C12" s="3"/>
-      <c r="F12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="2:12">
-      <c r="C13" s="3"/>
-      <c r="F13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="2:12">
-      <c r="C14" s="3"/>
-      <c r="F14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="2:12">
-      <c r="C15" s="3"/>
-      <c r="E15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="I15" s="7"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="2:12">
-      <c r="C16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="I16" s="7"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="3:15">
-      <c r="C17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="I17" s="7"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="3:15">
-      <c r="C18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="I18" s="7"/>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="3:15">
-      <c r="C19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="I19" s="7"/>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="3:15">
-      <c r="C20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="I20" s="7"/>
-      <c r="L20" s="3"/>
-      <c r="O20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15">
-      <c r="C21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="I21" s="7"/>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="3:15">
-      <c r="C22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="I22" s="7"/>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="3:15">
-      <c r="C23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="I23" s="7"/>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="3:15">
-      <c r="C24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="I24" s="7"/>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="3:15">
-      <c r="C25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="I25" s="7"/>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="3:15">
-      <c r="C26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="I26" s="7"/>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="3:15">
-      <c r="C27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="I27" s="7"/>
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="3:15">
-      <c r="C28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="3:15">
-      <c r="C29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="34" spans="12:12">
-      <c r="L34" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="12:12">
-      <c r="L35" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="12:12">
-      <c r="L36" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="12:12">
-      <c r="L37" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="12:12">
-      <c r="L38" s="6"/>
-    </row>
-    <row r="39" spans="12:12">
-      <c r="L39" s="7"/>
-    </row>
-    <row r="40" spans="12:12">
-      <c r="L40" s="3"/>
-    </row>
-    <row r="41" spans="12:12">
-      <c r="L41" s="4"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19FBDA2-FF85-45FB-B4CE-107905DAFA5C}">
-  <dimension ref="B2:N55"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -3052,40 +2151,40 @@
   <sheetData>
     <row r="2" spans="2:14">
       <c r="H2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="2:14">
       <c r="H3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="N3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:14">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:14" ht="37.5">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N5" s="9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:14">
@@ -3114,7 +2213,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="4:5">
@@ -3122,7 +2221,7 @@
         <v>24</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="4:5">
@@ -3130,12 +2229,12 @@
         <v>32</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="4:5">
       <c r="D21" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E21" s="5"/>
     </row>
@@ -3156,7 +2255,7 @@
     </row>
     <row r="27" spans="4:5">
       <c r="E27" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="4:5">
@@ -3173,6 +2272,11 @@
     </row>
     <row r="32" spans="4:5">
       <c r="E32" s="4"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="E35" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:5">
       <c r="E37" s="1" t="s">
@@ -3186,45 +2290,47 @@
     </row>
     <row r="39" spans="2:5">
       <c r="E39" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="E40" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="E41" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="E42" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="2:5">
       <c r="E43" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="2:5">
-      <c r="B44" s="8"/>
       <c r="E44" s="7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="2:5">
+      <c r="B45" s="8"/>
       <c r="E45" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="2:5">
-      <c r="E46" s="6"/>
+      <c r="E46" s="7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="47" spans="2:5">
-      <c r="E47" s="7"/>
+      <c r="E47" s="6"/>
     </row>
     <row r="48" spans="2:5">
       <c r="E48" s="7"/>
@@ -3233,26 +2339,29 @@
       <c r="E49" s="7"/>
     </row>
     <row r="50" spans="5:5">
-      <c r="E50" s="11" t="s">
-        <v>21</v>
-      </c>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="5:5">
-      <c r="E51" s="3"/>
+      <c r="E51" s="11" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="52" spans="5:5">
       <c r="E52" s="3"/>
     </row>
     <row r="53" spans="5:5">
-      <c r="E53" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="E53" s="3"/>
     </row>
     <row r="54" spans="5:5">
-      <c r="E54" s="3"/>
+      <c r="E54" s="10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="55" spans="5:5">
-      <c r="E55" s="4"/>
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="5:5">
+      <c r="E56" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
feat: introduce deallocate() of alloc_only_chamber class
</commit_message>
<xml_diff>
--- a/libalconcurrent/doc/alloc_only_allocator.xlsx
+++ b/libalconcurrent/doc/alloc_only_allocator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\alpha\work\alpha_concurrent\libalconcurrent\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D60999D-425A-465A-82A4-A3B63A90C6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1A5EB2-ADD5-4B7A-970B-7CC7E985E4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>allocate_by_mmap()でOSからメモリ領域を確保</t>
     <rPh sb="26" eb="28">
@@ -93,23 +93,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>次の空き領域へオフセット(size_t)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>参照先候補スタックリストとしての次へのポインタ</t>
-    <rPh sb="0" eb="3">
-      <t>サンショウサキ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>コウホ</t>
-    </rPh>
-    <rPh sb="16" eb="17">
-      <t>ツギ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>free_room</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -118,31 +101,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>offset_into_the_allocated_memory_</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>(アライメントの合わせ込みのためのパディング領域)</t>
-    <rPh sb="8" eb="9">
-      <t>ア</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>リョウイキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>tail_padding</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>バックトレース情報(コンパイルオプション)</t>
-    <rPh sb="7" eb="9">
-      <t>ジョウホウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -155,6 +114,36 @@
   </si>
   <si>
     <t>std::atomic&lt;bool&gt; is_freeed_</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>magic number</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次の空き領域へオフセット(uintptr_t)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(アライメントの合わせ込みのためのパディング領域)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>このchopped roomが属するalloc_chamberへのポインタ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>← ここのアドレスを、要求されたアライメントに合わせる。</t>
+    <rPh sb="11" eb="13">
+      <t>ヨウキュウ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ア</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>p_alloc_in_room_</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -178,7 +167,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +188,11 @@
     </fill>
     <fill>
       <patternFill patternType="lightUp">
+        <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="lightDown">
         <bgColor theme="0" tint="-4.9989318521683403E-2"/>
       </patternFill>
     </fill>
@@ -280,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -299,6 +293,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -442,7 +437,7 @@
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>132521</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -882,7 +877,7 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2371725</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -938,13 +933,13 @@
       <xdr:col>2</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>219074</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -959,8 +954,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4248150" y="9772649"/>
-          <a:ext cx="438150" cy="923925"/>
+          <a:off x="4248150" y="10010775"/>
+          <a:ext cx="438150" cy="695325"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -1015,7 +1010,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3267075" y="9848850"/>
+          <a:off x="3267075" y="10325100"/>
           <a:ext cx="975139" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1056,9 +1051,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
+      <xdr:colOff>895350</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
+      <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1066254" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -1074,7 +1069,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1619250" y="10448925"/>
+          <a:off x="1581150" y="11172825"/>
           <a:ext cx="1066254" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1115,15 +1110,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>28577</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>219076</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>209551</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1138,8 +1133,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4257675" y="10506077"/>
-          <a:ext cx="438150" cy="904874"/>
+          <a:off x="3981450" y="10753725"/>
+          <a:ext cx="438150" cy="1600201"/>
         </a:xfrm>
         <a:prstGeom prst="leftBrace">
           <a:avLst>
@@ -1176,11 +1171,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2409825</xdr:colOff>
+      <xdr:colOff>2314575</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1225015" cy="264560"/>
+    <xdr:ext cx="1008674" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="14" name="テキスト ボックス 13">
@@ -1194,8 +1189,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3095625" y="10810875"/>
-          <a:ext cx="1225015" cy="264560"/>
+          <a:off x="3000375" y="11534775"/>
+          <a:ext cx="1008674" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1224,7 +1219,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>allocated memory</a:t>
+            <a:t>alloc_in_room</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
@@ -1236,13 +1231,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>28577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1297,7 +1292,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2409825</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1313180" cy="1445011"/>
@@ -1400,7 +1395,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>2143125</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1415,8 +1410,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11668125" y="9563100"/>
-          <a:ext cx="276225" cy="2114550"/>
+          <a:off x="11668125" y="10039350"/>
+          <a:ext cx="276225" cy="2524125"/>
         </a:xfrm>
         <a:prstGeom prst="rightBrace">
           <a:avLst>
@@ -1453,7 +1448,7 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2181225</xdr:colOff>
+      <xdr:colOff>2152650</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
@@ -1471,7 +1466,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11982450" y="10477500"/>
+          <a:off x="11953875" y="11191875"/>
           <a:ext cx="1141531" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1592,14 +1587,14 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1614,8 +1609,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9163050" y="9629775"/>
-          <a:ext cx="409575" cy="933450"/>
+          <a:off x="9163050" y="10382250"/>
+          <a:ext cx="409575" cy="447675"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1702,89 +1697,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4773486" cy="328423"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="テキスト ボックス 22">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72FB9630-2D62-532A-6496-70CD6F87D7C9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9639300" y="9648825"/>
-          <a:ext cx="4773486" cy="328423"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>offset_into_the_allocated_memory_</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
-            <a:t>= room_boader</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-            <a:t>の</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>先頭からのオフセット</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -1863,6 +1775,367 @@
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
             <a:t>化できると思われる。</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2867025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="左中かっこ 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3446ECCB-C28B-41B0-B124-FAADEA6E1BB1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3552825" y="3848100"/>
+          <a:ext cx="438150" cy="3981450"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 40942"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1028808" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="テキスト ボックス 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{522AF726-04F7-4228-897A-14DBF27DA59F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2381250" y="5715000"/>
+          <a:ext cx="1028808" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ja-JP" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>alloc_chamber</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2581274</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104773</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400048</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114298</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="フリーフォーム: 図形 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{815C3F2B-869A-459C-98AE-646AED1804E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3267074" y="8915398"/>
+          <a:ext cx="1400174" cy="2390775"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="connsiteX0" fmla="*/ 28575 w 200025"/>
+            <a:gd name="connsiteY0" fmla="*/ 0 h 514350"/>
+            <a:gd name="connsiteX1" fmla="*/ 200025 w 200025"/>
+            <a:gd name="connsiteY1" fmla="*/ 114300 h 514350"/>
+            <a:gd name="connsiteX2" fmla="*/ 200025 w 200025"/>
+            <a:gd name="connsiteY2" fmla="*/ 409575 h 514350"/>
+            <a:gd name="connsiteX3" fmla="*/ 133350 w 200025"/>
+            <a:gd name="connsiteY3" fmla="*/ 514350 h 514350"/>
+            <a:gd name="connsiteX4" fmla="*/ 0 w 200025"/>
+            <a:gd name="connsiteY4" fmla="*/ 514350 h 514350"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX0" y="connsiteY0"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX1" y="connsiteY1"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX2" y="connsiteY2"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX3" y="connsiteY3"/>
+            </a:cxn>
+            <a:cxn ang="0">
+              <a:pos x="connsiteX4" y="connsiteY4"/>
+            </a:cxn>
+          </a:cxnLst>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="200025" h="514350">
+              <a:moveTo>
+                <a:pt x="28575" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="200025" y="114300"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="200025" y="409575"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="133350" y="514350"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="514350"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1225015" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="テキスト ボックス 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E6AC528-009B-459B-872D-696AA13D13E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5553075" y="11734800"/>
+          <a:ext cx="1225015" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>allocated memory</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="左中かっこ 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0E983D2-F31A-4081-8E45-85AE237E91D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5029200" y="11458576"/>
+          <a:ext cx="438150" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 40942"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2134,10 +2407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A19FBDA2-FF85-45FB-B4CE-107905DAFA5C}">
-  <dimension ref="B2:N56"/>
+  <dimension ref="B2:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2197,7 +2470,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="4:5">
@@ -2205,7 +2478,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="4:5">
@@ -2213,7 +2486,7 @@
         <v>16</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="4:5">
@@ -2221,7 +2494,7 @@
         <v>24</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="4:5">
@@ -2229,12 +2502,12 @@
         <v>32</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="4:5">
       <c r="D21" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E21" s="5"/>
     </row>
@@ -2255,7 +2528,7 @@
     </row>
     <row r="27" spans="4:5">
       <c r="E27" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="4:5">
@@ -2273,95 +2546,104 @@
     <row r="32" spans="4:5">
       <c r="E32" s="4"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:7">
       <c r="E35" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:7">
       <c r="E37" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="E38" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5">
-      <c r="E38" s="2" t="s">
+    <row r="39" spans="2:7">
+      <c r="E39" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:5">
-      <c r="E39" s="2" t="s">
+    <row r="40" spans="2:7">
+      <c r="E40" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="E41" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="E42" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
-      <c r="E40" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5">
-      <c r="E41" s="2" t="s">
+    <row r="43" spans="2:7">
+      <c r="E43" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="E44" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
-      <c r="E42" s="6" t="s">
+    <row r="45" spans="2:7">
+      <c r="B45" s="8"/>
+      <c r="E45" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
-      <c r="E43" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5">
-      <c r="E44" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5">
-      <c r="B45" s="8"/>
-      <c r="E45" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="2:7">
+      <c r="B46" s="8"/>
       <c r="E46" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="2:5">
-      <c r="E48" s="7"/>
+    <row r="47" spans="2:7">
+      <c r="E47" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="E48" s="12"/>
+      <c r="G48" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="49" spans="5:5">
-      <c r="E49" s="7"/>
+      <c r="E49" s="12"/>
     </row>
     <row r="50" spans="5:5">
-      <c r="E50" s="7"/>
+      <c r="E50" s="12"/>
     </row>
     <row r="51" spans="5:5">
-      <c r="E51" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="E51" s="12"/>
     </row>
     <row r="52" spans="5:5">
-      <c r="E52" s="3"/>
+      <c r="E52" s="11" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="53" spans="5:5">
       <c r="E53" s="3"/>
     </row>
     <row r="54" spans="5:5">
-      <c r="E54" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="E54" s="3"/>
     </row>
     <row r="55" spans="5:5">
-      <c r="E55" s="3"/>
+      <c r="E55" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="56" spans="5:5">
-      <c r="E56" s="4"/>
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="5:5">
+      <c r="E57" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>